<commit_message>
Add defect management assignments and update project file
Added multiple Excel and Word files related to defect management assignments, including HLRs, test cases, and theory documents. Also updated the DEFECT PROJECT 1.xlsx file in the project directory.
</commit_message>
<xml_diff>
--- a/Project/PROJECT 1/DEFECT PROJECT 1.xlsx
+++ b/Project/PROJECT 1/DEFECT PROJECT 1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9264" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="HLR" sheetId="1" r:id="rId1"/>
@@ -1219,9 +1219,6 @@
     <t>Defect Summary</t>
   </si>
   <si>
-    <t>Reproduced Step</t>
-  </si>
-  <si>
     <t>Defect Type</t>
   </si>
   <si>
@@ -1377,6 +1374,9 @@
   </si>
   <si>
     <t xml:space="preserve">when navigate with tab key not to see cursor on button </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Step</t>
   </si>
 </sst>
 </file>
@@ -10703,7 +10703,7 @@
         <v>3</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E2" s="55" t="s">
         <v>85</v>
@@ -11228,13 +11228,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
+    <col min="1" max="1" width="11.88671875" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" customWidth="1"/>
     <col min="3" max="3" width="20.6640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
@@ -11250,7 +11250,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="23" customFormat="1" ht="31.2">
       <c r="A1" s="45" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B1" s="20" t="s">
         <v>74</v>
@@ -11259,31 +11259,31 @@
         <v>287</v>
       </c>
       <c r="D1" s="20" t="s">
-        <v>288</v>
+        <v>340</v>
       </c>
       <c r="E1" s="21" t="s">
         <v>79</v>
       </c>
       <c r="F1" s="22" t="s">
+        <v>288</v>
+      </c>
+      <c r="G1" s="20" t="s">
         <v>289</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>290</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="I1" s="21" t="s">
         <v>291</v>
       </c>
-      <c r="I1" s="21" t="s">
-        <v>292</v>
-      </c>
       <c r="J1" s="24" t="s">
+        <v>293</v>
+      </c>
+      <c r="K1" s="24" t="s">
         <v>294</v>
       </c>
-      <c r="K1" s="24" t="s">
+      <c r="L1" s="24" t="s">
         <v>295</v>
-      </c>
-      <c r="L1" s="24" t="s">
-        <v>296</v>
       </c>
       <c r="M1" s="24" t="s">
         <v>82</v>
@@ -11306,13 +11306,13 @@
         <v>90</v>
       </c>
       <c r="F2" s="47" t="s">
+        <v>297</v>
+      </c>
+      <c r="G2" s="47" t="s">
         <v>298</v>
       </c>
-      <c r="G2" s="47" t="s">
+      <c r="H2" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H2" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I2" s="49" t="s">
         <v>91</v>
@@ -11321,13 +11321,13 @@
         <v>92</v>
       </c>
       <c r="K2" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L2" s="25" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="M2" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N2" s="50"/>
     </row>
@@ -11348,13 +11348,13 @@
         <v>95</v>
       </c>
       <c r="F3" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G3" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H3" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H3" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I3" s="49" t="s">
         <v>96</v>
@@ -11363,13 +11363,13 @@
         <v>97</v>
       </c>
       <c r="K3" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L3" s="25" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="M3" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N3" s="50"/>
     </row>
@@ -11390,13 +11390,13 @@
         <v>99</v>
       </c>
       <c r="F4" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G4" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H4" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H4" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I4" s="49" t="s">
         <v>96</v>
@@ -11405,13 +11405,13 @@
         <v>100</v>
       </c>
       <c r="K4" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L4" s="25" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="M4" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N4" s="50"/>
     </row>
@@ -11432,13 +11432,13 @@
         <v>101</v>
       </c>
       <c r="F5" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G5" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H5" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H5" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I5" s="49" t="s">
         <v>96</v>
@@ -11447,13 +11447,13 @@
         <v>100</v>
       </c>
       <c r="K5" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="M5" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N5" s="50"/>
     </row>
@@ -11474,13 +11474,13 @@
         <v>105</v>
       </c>
       <c r="F6" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G6" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H6" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H6" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I6" s="49" t="s">
         <v>96</v>
@@ -11489,13 +11489,13 @@
         <v>100</v>
       </c>
       <c r="K6" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L6" s="25" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="M6" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N6" s="50"/>
     </row>
@@ -11516,13 +11516,13 @@
         <v>107</v>
       </c>
       <c r="F7" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G7" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H7" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H7" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I7" s="49" t="s">
         <v>96</v>
@@ -11531,13 +11531,13 @@
         <v>108</v>
       </c>
       <c r="K7" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L7" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M7" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N7" s="50"/>
     </row>
@@ -11558,13 +11558,13 @@
         <v>110</v>
       </c>
       <c r="F8" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G8" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H8" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H8" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I8" s="49" t="s">
         <v>96</v>
@@ -11573,13 +11573,13 @@
         <v>108</v>
       </c>
       <c r="K8" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L8" s="25" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="M8" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N8" s="50"/>
     </row>
@@ -11600,13 +11600,13 @@
         <v>111</v>
       </c>
       <c r="F9" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G9" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H9" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H9" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I9" s="49" t="s">
         <v>96</v>
@@ -11615,13 +11615,13 @@
         <v>100</v>
       </c>
       <c r="K9" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L9" s="25" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="M9" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N9" s="50"/>
     </row>
@@ -11642,13 +11642,13 @@
         <v>114</v>
       </c>
       <c r="F10" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G10" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H10" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H10" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I10" s="49" t="s">
         <v>96</v>
@@ -11657,13 +11657,13 @@
         <v>100</v>
       </c>
       <c r="K10" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L10" s="25" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="M10" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N10" s="50"/>
     </row>
@@ -11684,13 +11684,13 @@
         <v>115</v>
       </c>
       <c r="F11" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G11" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H11" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H11" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I11" s="49" t="s">
         <v>96</v>
@@ -11699,13 +11699,13 @@
         <v>100</v>
       </c>
       <c r="K11" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L11" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M11" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N11" s="50"/>
     </row>
@@ -11726,13 +11726,13 @@
         <v>117</v>
       </c>
       <c r="F12" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G12" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H12" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H12" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I12" s="49" t="s">
         <v>96</v>
@@ -11741,13 +11741,13 @@
         <v>100</v>
       </c>
       <c r="K12" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L12" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M12" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N12" s="50"/>
     </row>
@@ -11768,13 +11768,13 @@
         <v>117</v>
       </c>
       <c r="F13" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G13" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H13" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H13" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I13" s="49" t="s">
         <v>96</v>
@@ -11783,13 +11783,13 @@
         <v>100</v>
       </c>
       <c r="K13" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L13" s="25" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="M13" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N13" s="50"/>
     </row>
@@ -11810,13 +11810,13 @@
         <v>119</v>
       </c>
       <c r="F14" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G14" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H14" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H14" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I14" s="49" t="s">
         <v>96</v>
@@ -11825,13 +11825,13 @@
         <v>100</v>
       </c>
       <c r="K14" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L14" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M14" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N14" s="50"/>
     </row>
@@ -11852,13 +11852,13 @@
         <v>120</v>
       </c>
       <c r="F15" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G15" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H15" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H15" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I15" s="49" t="s">
         <v>96</v>
@@ -11867,13 +11867,13 @@
         <v>122</v>
       </c>
       <c r="K15" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L15" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M15" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N15" s="50"/>
     </row>
@@ -11894,13 +11894,13 @@
         <v>121</v>
       </c>
       <c r="F16" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G16" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H16" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H16" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I16" s="49" t="s">
         <v>96</v>
@@ -11909,13 +11909,13 @@
         <v>123</v>
       </c>
       <c r="K16" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L16" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M16" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N16" s="50"/>
     </row>
@@ -11936,13 +11936,13 @@
         <v>126</v>
       </c>
       <c r="F17" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G17" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H17" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H17" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I17" s="49" t="s">
         <v>96</v>
@@ -11951,13 +11951,13 @@
         <v>127</v>
       </c>
       <c r="K17" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L17" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M17" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N17" s="50"/>
     </row>
@@ -11978,13 +11978,13 @@
         <v>131</v>
       </c>
       <c r="F18" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G18" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H18" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H18" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I18" s="49" t="s">
         <v>96</v>
@@ -11993,13 +11993,13 @@
         <v>132</v>
       </c>
       <c r="K18" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L18" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M18" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N18" s="50"/>
     </row>
@@ -12020,13 +12020,13 @@
         <v>135</v>
       </c>
       <c r="F19" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G19" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H19" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H19" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I19" s="49" t="s">
         <v>96</v>
@@ -12035,13 +12035,13 @@
         <v>123</v>
       </c>
       <c r="K19" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L19" s="25" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="M19" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N19" s="50"/>
     </row>
@@ -12062,13 +12062,13 @@
         <v>136</v>
       </c>
       <c r="F20" s="47" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G20" s="47" t="s">
+        <v>298</v>
+      </c>
+      <c r="H20" s="47" t="s">
         <v>299</v>
-      </c>
-      <c r="H20" s="47" t="s">
-        <v>300</v>
       </c>
       <c r="I20" s="49" t="s">
         <v>96</v>
@@ -12077,13 +12077,13 @@
         <v>137</v>
       </c>
       <c r="K20" s="47" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="L20" s="25" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="M20" s="47" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="N20" s="50"/>
     </row>
@@ -12132,16 +12132,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36">
       <c r="A1" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="35" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>317</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="31.2">
@@ -12149,13 +12149,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="31" t="s">
+        <v>305</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>306</v>
       </c>
-      <c r="C2" s="38" t="s">
-        <v>307</v>
-      </c>
       <c r="D2" s="31" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="27" customFormat="1" ht="31.2">
@@ -12163,13 +12163,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="34" t="s">
+        <v>307</v>
+      </c>
+      <c r="C3" s="39" t="s">
         <v>308</v>
       </c>
-      <c r="C3" s="39" t="s">
-        <v>309</v>
-      </c>
       <c r="D3" s="31" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="26" customFormat="1" ht="31.2">
@@ -12177,13 +12177,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="34" t="s">
+        <v>309</v>
+      </c>
+      <c r="C4" s="40" t="s">
         <v>310</v>
       </c>
-      <c r="C4" s="40" t="s">
+      <c r="D4" s="33" t="s">
         <v>311</v>
-      </c>
-      <c r="D4" s="33" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="28" customFormat="1" ht="31.2">
@@ -12191,13 +12191,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="37" t="s">
+        <v>312</v>
+      </c>
+      <c r="C5" s="41" t="s">
+        <v>308</v>
+      </c>
+      <c r="D5" s="34" t="s">
         <v>313</v>
-      </c>
-      <c r="C5" s="41" t="s">
-        <v>309</v>
-      </c>
-      <c r="D5" s="34" t="s">
-        <v>314</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="15.6">
@@ -12270,7 +12270,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
@@ -12283,16 +12283,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="18">
       <c r="A1" s="42" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="42" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="C1" s="42" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="42" t="s">
         <v>317</v>
-      </c>
-      <c r="D1" s="42" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="75" customFormat="1" ht="31.2">
@@ -12300,13 +12300,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" s="74" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
     </row>
     <row r="3" spans="1:4" s="75" customFormat="1" ht="31.2">
@@ -12314,13 +12314,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="43" t="s">
+        <v>323</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>324</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="D3" s="74" t="s">
         <v>325</v>
-      </c>
-      <c r="D3" s="74" t="s">
-        <v>326</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="75" customFormat="1" ht="31.2">
@@ -12328,13 +12328,13 @@
         <v>3</v>
       </c>
       <c r="B4" s="31" t="s">
+        <v>326</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>308</v>
+      </c>
+      <c r="D4" s="74" t="s">
         <v>327</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>309</v>
-      </c>
-      <c r="D4" s="74" t="s">
-        <v>328</v>
       </c>
     </row>
   </sheetData>
@@ -12365,16 +12365,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="36">
       <c r="A1" s="35" t="s">
+        <v>314</v>
+      </c>
+      <c r="B1" s="35" t="s">
         <v>315</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="C1" s="35" t="s">
         <v>316</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="D1" s="35" t="s">
         <v>317</v>
-      </c>
-      <c r="D1" s="35" t="s">
-        <v>318</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.6">
@@ -12382,13 +12382,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="43" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D2" s="43" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="31.2">
@@ -12396,13 +12396,13 @@
         <v>2</v>
       </c>
       <c r="B3" s="43" t="s">
+        <v>334</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>335</v>
       </c>
-      <c r="C3" s="44" t="s">
+      <c r="D3" s="31" t="s">
         <v>336</v>
-      </c>
-      <c r="D3" s="31" t="s">
-        <v>337</v>
       </c>
     </row>
   </sheetData>

</xml_diff>